<commit_message>
Added New work types
</commit_message>
<xml_diff>
--- a/DaysOff/demo.xlsx
+++ b/DaysOff/demo.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve"> DATE</t>
   </si>
   <si>
-    <t>10/03/2020</t>
+    <t>11/03/2020</t>
   </si>
   <si>
     <t xml:space="preserve"> OVER ROTA</t>
@@ -50,22 +50,13 @@
     <t xml:space="preserve">  KITCHEN  </t>
   </si>
   <si>
-    <t>MahaDeva PM</t>
-  </si>
-  <si>
-    <t>MahaDeva AM</t>
-  </si>
-  <si>
-    <t>Adam PM</t>
-  </si>
-  <si>
-    <t>Adam AM</t>
-  </si>
-  <si>
-    <t>Supriti AM</t>
-  </si>
-  <si>
-    <t>Supriti PM</t>
+    <t>MahaDeva</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Supriti</t>
   </si>
   <si>
     <t>Anna</t>
@@ -210,7 +201,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.3176441192627" customWidth="1"/>
+    <col min="1" max="1" width="8.3193187713623" customWidth="1"/>
     <col min="2" max="2" width="15.0979623794556" customWidth="1"/>
     <col min="3" max="3" width="16.8727016448975" customWidth="1"/>
     <col min="4" max="4" width="10.776349067688" customWidth="1"/>
@@ -265,11 +256,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -279,11 +268,9 @@
       <c r="H3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -293,11 +280,9 @@
       <c r="H4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="A5" s="4"/>
       <c r="B5" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -309,7 +294,7 @@
     <row r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -321,7 +306,7 @@
     <row r="7">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -333,7 +318,7 @@
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -345,7 +330,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -357,7 +342,7 @@
     <row r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>

</xml_diff>

<commit_message>
added ownjobs worktype to excel export
</commit_message>
<xml_diff>
--- a/DaysOff/demo.xlsx
+++ b/DaysOff/demo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve"> DATE</t>
   </si>
@@ -50,28 +50,70 @@
     <t xml:space="preserve">  KITCHEN  </t>
   </si>
   <si>
+    <t>Adam PM</t>
+  </si>
+  <si>
+    <t>Navi</t>
+  </si>
+  <si>
     <t>MahaDeva</t>
   </si>
   <si>
-    <t>Adam</t>
+    <t>Mahi - OJ</t>
+  </si>
+  <si>
+    <t>Dganit</t>
   </si>
   <si>
     <t>Supriti</t>
   </si>
   <si>
+    <t>Neal</t>
+  </si>
+  <si>
+    <t>Khalsa - PR</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Anna AM</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>Adam - BY</t>
+  </si>
+  <si>
+    <t>Shakti</t>
+  </si>
+  <si>
+    <t>Anuka AM</t>
+  </si>
+  <si>
+    <t>Khalsa</t>
+  </si>
+  <si>
+    <t>Adam AM</t>
+  </si>
+  <si>
+    <t>Anna PM</t>
+  </si>
+  <si>
+    <t>Anuka PM</t>
+  </si>
+  <si>
+    <t>Mahi</t>
+  </si>
+  <si>
+    <t>RAP</t>
+  </si>
+  <si>
+    <t>Anuka - OJ</t>
+  </si>
+  <si>
     <t>Anna</t>
-  </si>
-  <si>
-    <t>Dganit</t>
-  </si>
-  <si>
-    <t>Shakti</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
@@ -198,10 +240,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.3193187713623" customWidth="1"/>
+    <col min="1" max="1" width="10.5261631011963" customWidth="1"/>
     <col min="2" max="2" width="15.0979623794556" customWidth="1"/>
     <col min="3" max="3" width="16.8727016448975" customWidth="1"/>
-    <col min="4" max="4" width="10.776349067688" customWidth="1"/>
+    <col min="4" max="4" width="10.8688907623291" customWidth="1"/>
     <col min="5" max="5" width="14.6318159103394" customWidth="1"/>
     <col min="6" max="6" width="13.9846811294556" customWidth="1"/>
     <col min="7" max="7" width="10.7503070831299" customWidth="1"/>
@@ -253,51 +295,65 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="B3" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="B4" s="7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="B5" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -307,9 +363,11 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -321,7 +379,7 @@
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -333,7 +391,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -345,7 +403,7 @@
     <row r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -356,7 +414,9 @@
     </row>
     <row r="11">
       <c r="A11" s="4"/>
-      <c r="B11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -366,7 +426,9 @@
     </row>
     <row r="12">
       <c r="A12" s="4"/>
-      <c r="B12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -376,7 +438,9 @@
     </row>
     <row r="13">
       <c r="A13" s="4"/>
-      <c r="B13" s="7"/>
+      <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -386,7 +450,9 @@
     </row>
     <row r="14">
       <c r="A14" s="4"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -427,9 +493,7 @@
     <row r="18">
       <c r="A18" s="4"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -439,22 +503,36 @@
     <row r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>14</v>
+      </c>
       <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="F19" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="H19" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="H20" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="4"/>

</xml_diff>

<commit_message>
added OHC tag in House Care col Excel
</commit_message>
<xml_diff>
--- a/DaysOff/demo.xlsx
+++ b/DaysOff/demo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve"> DATE</t>
   </si>
@@ -56,39 +56,42 @@
     <t>Navi</t>
   </si>
   <si>
+    <t>MahaDeva - OHC</t>
+  </si>
+  <si>
+    <t>Mahi - OJ</t>
+  </si>
+  <si>
+    <t>Dganit</t>
+  </si>
+  <si>
+    <t>Supriti</t>
+  </si>
+  <si>
+    <t>Neal</t>
+  </si>
+  <si>
+    <t>Khalsa - PR</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Anna AM</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>Adam - BY</t>
+  </si>
+  <si>
+    <t>Shakti</t>
+  </si>
+  <si>
     <t>MahaDeva</t>
   </si>
   <si>
-    <t>Mahi - OJ</t>
-  </si>
-  <si>
-    <t>Dganit</t>
-  </si>
-  <si>
-    <t>Supriti</t>
-  </si>
-  <si>
-    <t>Neal</t>
-  </si>
-  <si>
-    <t>Khalsa - PR</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>Anna AM</t>
-  </si>
-  <si>
-    <t>Mel</t>
-  </si>
-  <si>
-    <t>Adam - BY</t>
-  </si>
-  <si>
-    <t>Shakti</t>
-  </si>
-  <si>
     <t>Anuka AM</t>
   </si>
   <si>
@@ -113,7 +116,7 @@
     <t>Anuka - OJ</t>
   </si>
   <si>
-    <t>Anna</t>
+    <t>Anna - OHC</t>
   </si>
 </sst>
 </file>
@@ -353,7 +356,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -364,10 +367,10 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -379,7 +382,7 @@
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -391,7 +394,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -415,7 +418,7 @@
     <row r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -439,7 +442,7 @@
     <row r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -451,7 +454,7 @@
     <row r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -507,22 +510,22 @@
         <v>16</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>

</xml_diff>

<commit_message>
Added MC to excel export
</commit_message>
<xml_diff>
--- a/DaysOff/demo.xlsx
+++ b/DaysOff/demo.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve"> DATE</t>
   </si>
   <si>
-    <t>12/03/2020</t>
+    <t>16/03/2020</t>
   </si>
   <si>
     <t xml:space="preserve"> OVER ROTA</t>
@@ -50,73 +50,73 @@
     <t xml:space="preserve">  KITCHEN  </t>
   </si>
   <si>
-    <t>Adam PM</t>
+    <t>MahaDeva AM</t>
   </si>
   <si>
     <t>Navi</t>
   </si>
   <si>
+    <t>Mahi</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Shakti - OJ</t>
+  </si>
+  <si>
+    <t>Ben - MC</t>
+  </si>
+  <si>
+    <t>Khalsa</t>
+  </si>
+  <si>
+    <t>Neal</t>
+  </si>
+  <si>
+    <t>Adam - OHC</t>
+  </si>
+  <si>
+    <t>Supriti</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>Dganit AM</t>
+  </si>
+  <si>
+    <t>MahaDeva PM</t>
+  </si>
+  <si>
+    <t>Anuka AM</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Dganit PM</t>
+  </si>
+  <si>
+    <t>Shakti</t>
+  </si>
+  <si>
+    <t>Anuka PM</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>RAP</t>
+  </si>
+  <si>
     <t>MahaDeva - OHC</t>
   </si>
   <si>
-    <t>Mahi - OJ</t>
-  </si>
-  <si>
     <t>Dganit</t>
   </si>
   <si>
-    <t>Supriti</t>
-  </si>
-  <si>
-    <t>Neal</t>
-  </si>
-  <si>
-    <t>Khalsa - PR</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t>Anna AM</t>
-  </si>
-  <si>
-    <t>Mel</t>
-  </si>
-  <si>
-    <t>Adam - BY</t>
-  </si>
-  <si>
-    <t>Shakti</t>
-  </si>
-  <si>
-    <t>MahaDeva</t>
-  </si>
-  <si>
-    <t>Anuka AM</t>
-  </si>
-  <si>
-    <t>Khalsa</t>
-  </si>
-  <si>
-    <t>Adam AM</t>
-  </si>
-  <si>
-    <t>Anna PM</t>
-  </si>
-  <si>
-    <t>Anuka PM</t>
-  </si>
-  <si>
-    <t>Mahi</t>
-  </si>
-  <si>
-    <t>RAP</t>
-  </si>
-  <si>
-    <t>Anuka - OJ</t>
-  </si>
-  <si>
-    <t>Anna - OHC</t>
+    <t>Anuka - MC</t>
   </si>
 </sst>
 </file>
@@ -243,10 +243,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5261631011963" customWidth="1"/>
+    <col min="1" max="1" width="14.4516658782959" customWidth="1"/>
     <col min="2" max="2" width="15.0979623794556" customWidth="1"/>
     <col min="3" max="3" width="16.8727016448975" customWidth="1"/>
-    <col min="4" max="4" width="10.8688907623291" customWidth="1"/>
+    <col min="4" max="4" width="10.776349067688" customWidth="1"/>
     <col min="5" max="5" width="14.6318159103394" customWidth="1"/>
     <col min="6" max="6" width="13.9846811294556" customWidth="1"/>
     <col min="7" max="7" width="10.7503070831299" customWidth="1"/>
@@ -308,32 +308,32 @@
         <v>14</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="H4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
@@ -345,18 +345,16 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -367,10 +365,10 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -382,7 +380,7 @@
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -394,7 +392,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -406,7 +404,7 @@
     <row r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -418,7 +416,7 @@
     <row r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -430,7 +428,7 @@
     <row r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -442,7 +440,7 @@
     <row r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="7" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -454,7 +452,7 @@
     <row r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -507,34 +505,30 @@
       <c r="A19" s="4"/>
       <c r="B19" s="7"/>
       <c r="C19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
-      <c r="F20" s="7" t="s">
-        <v>19</v>
-      </c>
+      <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">

</xml_diff>

<commit_message>
fixed bug excel col to narrow when no one off for day
</commit_message>
<xml_diff>
--- a/DaysOff/demo.xlsx
+++ b/DaysOff/demo.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve"> DATE</t>
   </si>
   <si>
-    <t>16/03/2020</t>
+    <t>25/03/2020</t>
   </si>
   <si>
     <t xml:space="preserve"> OVER ROTA</t>
@@ -50,73 +50,49 @@
     <t xml:space="preserve">  KITCHEN  </t>
   </si>
   <si>
-    <t>MahaDeva AM</t>
+    <t>___________</t>
   </si>
   <si>
     <t>Navi</t>
   </si>
   <si>
+    <t>Shakti - OJ</t>
+  </si>
+  <si>
+    <t>Neal</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>MahaDeva</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Supriti</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Dganit</t>
+  </si>
+  <si>
+    <t>Shakti</t>
+  </si>
+  <si>
+    <t>Anuka</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
     <t>Mahi</t>
   </si>
   <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>Shakti - OJ</t>
-  </si>
-  <si>
-    <t>Ben - MC</t>
-  </si>
-  <si>
-    <t>Khalsa</t>
-  </si>
-  <si>
-    <t>Neal</t>
-  </si>
-  <si>
-    <t>Adam - OHC</t>
-  </si>
-  <si>
-    <t>Supriti</t>
-  </si>
-  <si>
-    <t>Mel</t>
-  </si>
-  <si>
-    <t>Dganit AM</t>
-  </si>
-  <si>
-    <t>MahaDeva PM</t>
-  </si>
-  <si>
-    <t>Anuka AM</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Dganit PM</t>
-  </si>
-  <si>
-    <t>Shakti</t>
-  </si>
-  <si>
-    <t>Anuka PM</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
     <t>RAP</t>
-  </si>
-  <si>
-    <t>MahaDeva - OHC</t>
-  </si>
-  <si>
-    <t>Dganit</t>
-  </si>
-  <si>
-    <t>Anuka - MC</t>
   </si>
 </sst>
 </file>
@@ -243,7 +219,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.4516658782959" customWidth="1"/>
+    <col min="1" max="1" width="13.2403564453125" customWidth="1"/>
     <col min="2" max="2" width="15.0979623794556" customWidth="1"/>
     <col min="3" max="3" width="16.8727016448975" customWidth="1"/>
     <col min="4" max="4" width="10.776349067688" customWidth="1"/>
@@ -304,31 +280,21 @@
       <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>20</v>
-      </c>
+      <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -336,11 +302,9 @@
       <c r="H4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="A5" s="4"/>
       <c r="B5" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -350,11 +314,9 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="A6" s="4"/>
       <c r="B6" s="7" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -364,11 +326,9 @@
       <c r="H6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -380,7 +340,7 @@
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -392,7 +352,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -404,7 +364,7 @@
     <row r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -416,7 +376,7 @@
     <row r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -428,7 +388,7 @@
     <row r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -440,7 +400,7 @@
     <row r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -452,7 +412,7 @@
     <row r="14">
       <c r="A14" s="4"/>
       <c r="B14" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -463,7 +423,9 @@
     </row>
     <row r="15">
       <c r="A15" s="4"/>
-      <c r="B15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -504,20 +466,12 @@
     <row r="19">
       <c r="A19" s="4"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="H19" s="8"/>
     </row>
     <row r="20">
       <c r="A20" s="4"/>
@@ -527,9 +481,7 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21">
       <c r="A21" s="4"/>

</xml_diff>

<commit_message>
Rescaked page size for excel export
</commit_message>
<xml_diff>
--- a/DaysOff/demo.xlsx
+++ b/DaysOff/demo.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <t>Sunday</t>
+    <t xml:space="preserve">  Sunday</t>
   </si>
   <si>
     <t>29/03/2020</t>
@@ -213,14 +213,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Added override holiday day selection
</commit_message>
<xml_diff>
--- a/DaysOff/demo.xlsx
+++ b/DaysOff/demo.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <t xml:space="preserve">  Sunday</t>
-  </si>
-  <si>
-    <t>29/03/2020</t>
+    <t xml:space="preserve">  Wednesday</t>
+  </si>
+  <si>
+    <t>01/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve"> OVER ROTA</t>
@@ -50,28 +50,28 @@
     <t xml:space="preserve">  KITCHEN  </t>
   </si>
   <si>
+    <t>Supriti</t>
+  </si>
+  <si>
+    <t>Navi</t>
+  </si>
+  <si>
+    <t>Shakti</t>
+  </si>
+  <si>
+    <t>Neal</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>MahaDeva</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
     <t>Anna</t>
-  </si>
-  <si>
-    <t>Navi</t>
-  </si>
-  <si>
-    <t>Shakti</t>
-  </si>
-  <si>
-    <t>Neal</t>
-  </si>
-  <si>
-    <t>Mel</t>
-  </si>
-  <si>
-    <t>MahaDeva</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Supriti</t>
   </si>
   <si>
     <t>Dganit</t>
@@ -217,10 +217,10 @@
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Added View called Rota to print spreadsheet for rota. ALso added migrations
</commit_message>
<xml_diff>
--- a/DaysOff/demo.xlsx
+++ b/DaysOff/demo.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">  Wednesday</t>
-  </si>
-  <si>
-    <t>01/04/2020</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">  Tuesday</t>
+  </si>
+  <si>
+    <t>07/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve"> OVER ROTA</t>
@@ -50,31 +50,28 @@
     <t xml:space="preserve">  KITCHEN  </t>
   </si>
   <si>
+    <t>___________</t>
+  </si>
+  <si>
+    <t>Navi</t>
+  </si>
+  <si>
+    <t>Neal</t>
+  </si>
+  <si>
+    <t>Mel</t>
+  </si>
+  <si>
+    <t>MahaDeva</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
     <t>Supriti</t>
   </si>
   <si>
-    <t>Navi</t>
-  </si>
-  <si>
-    <t>Shakti</t>
-  </si>
-  <si>
-    <t>Neal</t>
-  </si>
-  <si>
-    <t>Mel</t>
-  </si>
-  <si>
-    <t>MahaDeva</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
     <t>Anna</t>
-  </si>
-  <si>
-    <t>Dganit</t>
   </si>
   <si>
     <t>Anuka</t>
@@ -282,11 +279,9 @@
       <c r="H3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -298,7 +293,7 @@
     <row r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -310,7 +305,7 @@
     <row r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -322,7 +317,7 @@
     <row r="7">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -334,7 +329,7 @@
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -346,7 +341,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -358,7 +353,7 @@
     <row r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -370,7 +365,7 @@
     <row r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -382,7 +377,7 @@
     <row r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -394,7 +389,7 @@
     <row r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>

</xml_diff>

<commit_message>
Fixed rota print date bug
</commit_message>
<xml_diff>
--- a/DaysOff/demo.xlsx
+++ b/DaysOff/demo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve">  Tuesday</t>
   </si>
@@ -50,28 +50,37 @@
     <t xml:space="preserve">  KITCHEN  </t>
   </si>
   <si>
-    <t>___________</t>
+    <t>MahaDeva PM</t>
   </si>
   <si>
     <t>Navi</t>
   </si>
   <si>
+    <t>MahaDeva - OHC</t>
+  </si>
+  <si>
     <t>Neal</t>
   </si>
   <si>
+    <t>Adam</t>
+  </si>
+  <si>
     <t>Mel</t>
   </si>
   <si>
-    <t>MahaDeva</t>
-  </si>
-  <si>
-    <t>Adam</t>
+    <t>MahaDeva AM</t>
   </si>
   <si>
     <t>Supriti</t>
   </si>
   <si>
     <t>Anna</t>
+  </si>
+  <si>
+    <t>Dganit</t>
+  </si>
+  <si>
+    <t>Shakti</t>
   </si>
   <si>
     <t>Anuka</t>
@@ -271,7 +280,9 @@
       <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -281,9 +292,11 @@
     <row r="4">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -293,7 +306,7 @@
     <row r="5">
       <c r="A5" s="4"/>
       <c r="B5" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -305,7 +318,7 @@
     <row r="6">
       <c r="A6" s="4"/>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -317,7 +330,7 @@
     <row r="7">
       <c r="A7" s="4"/>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -329,7 +342,7 @@
     <row r="8">
       <c r="A8" s="4"/>
       <c r="B8" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -341,7 +354,7 @@
     <row r="9">
       <c r="A9" s="4"/>
       <c r="B9" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -353,7 +366,7 @@
     <row r="10">
       <c r="A10" s="4"/>
       <c r="B10" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -365,7 +378,7 @@
     <row r="11">
       <c r="A11" s="4"/>
       <c r="B11" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -377,7 +390,7 @@
     <row r="12">
       <c r="A12" s="4"/>
       <c r="B12" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -389,7 +402,7 @@
     <row r="13">
       <c r="A13" s="4"/>
       <c r="B13" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -400,7 +413,9 @@
     </row>
     <row r="14">
       <c r="A14" s="4"/>
-      <c r="B14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -410,7 +425,9 @@
     </row>
     <row r="15">
       <c r="A15" s="4"/>
-      <c r="B15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>

</xml_diff>